<commit_message>
The big ball of mud part 99
http://www.laputan.org/pub/foote/mud.pdf
</commit_message>
<xml_diff>
--- a/Excel Models/Reinsurance/408.xlsx
+++ b/Excel Models/Reinsurance/408.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcelo.franceschini\OneDrive - GRANT THORNTON BRASIL\MMF\Python\ActuarialServices\Excel Models\Reinsurance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3298CFD8-8620-400F-A311-9E30C42E4BFC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{A232E031-650C-450F-92DF-581EA4477345}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{3298CFD8-8620-400F-A311-9E30C42E4BFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{917959B8-D736-41C9-A945-7A03325629B8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2E2AA8CA-46CF-4850-A02C-5678BABF5C29}"/>
   </bookViews>
@@ -256,7 +256,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-416]mmm\-yy;@"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
@@ -681,9 +682,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -763,9 +765,6 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -791,6 +790,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -807,9 +809,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="2" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1331,9 +1334,7 @@
   </sheetPr>
   <dimension ref="A1:BS1048576"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BD9" workbookViewId="0">
-      <selection activeCell="BP14" sqref="BP14"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="0" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1363,7 +1364,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36"/>
+      <c r="A1" s="35"/>
     </row>
     <row r="2" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:71" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1503,16 +1504,16 @@
       <c r="BS12" s="45"/>
     </row>
     <row r="13" spans="1:71" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="39" t="s">
+      <c r="D13" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="39" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="6" t="s">
@@ -3544,11 +3545,11 @@
       </c>
       <c r="H26" s="42"/>
       <c r="I26" s="42"/>
-      <c r="J26" s="31">
-        <f>SUM(J14:J25)</f>
-        <v>0</v>
-      </c>
-      <c r="K26" s="32">
+      <c r="J26" s="40">
+        <f>ROUND(SUM(J14:J25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="K26" s="31">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3557,11 +3558,11 @@
       </c>
       <c r="N26" s="42"/>
       <c r="O26" s="42"/>
-      <c r="P26" s="31">
-        <f>SUM(P14:P25)</f>
-        <v>0</v>
-      </c>
-      <c r="Q26" s="32">
+      <c r="P26" s="40">
+        <f>ROUND(SUM(P14:P25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
@@ -3570,11 +3571,11 @@
       </c>
       <c r="T26" s="42"/>
       <c r="U26" s="42"/>
-      <c r="V26" s="31">
-        <f>SUM(V14:V25)</f>
-        <v>0</v>
-      </c>
-      <c r="W26" s="32">
+      <c r="V26" s="40">
+        <f>ROUND(SUM(V14:V25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="W26" s="31">
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
@@ -3583,11 +3584,11 @@
       </c>
       <c r="Z26" s="42"/>
       <c r="AA26" s="42"/>
-      <c r="AB26" s="31">
-        <f>SUM(AB14:AB25)</f>
-        <v>0</v>
-      </c>
-      <c r="AC26" s="32">
+      <c r="AB26" s="40">
+        <f>ROUND(SUM(AB14:AB25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="AC26" s="31">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
@@ -3596,11 +3597,11 @@
       </c>
       <c r="AF26" s="42"/>
       <c r="AG26" s="42"/>
-      <c r="AH26" s="31">
-        <f>SUM(AH14:AH25)</f>
-        <v>0</v>
-      </c>
-      <c r="AI26" s="32">
+      <c r="AH26" s="40">
+        <f>ROUND(SUM(AH14:AH25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="AI26" s="31">
         <f t="shared" si="16"/>
         <v>0</v>
       </c>
@@ -3609,11 +3610,11 @@
       </c>
       <c r="AL26" s="42"/>
       <c r="AM26" s="42"/>
-      <c r="AN26" s="31">
-        <f>SUM(AN14:AN25)</f>
-        <v>0</v>
-      </c>
-      <c r="AO26" s="32">
+      <c r="AN26" s="40">
+        <f>ROUND(SUM(AN14:AN25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="AO26" s="31">
         <f t="shared" si="18"/>
         <v>0</v>
       </c>
@@ -3622,11 +3623,11 @@
       </c>
       <c r="AR26" s="42"/>
       <c r="AS26" s="42"/>
-      <c r="AT26" s="31">
-        <f>SUM(AT14:AT25)</f>
-        <v>0</v>
-      </c>
-      <c r="AU26" s="32">
+      <c r="AT26" s="40">
+        <f>ROUND(SUM(AT14:AT25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="AU26" s="31">
         <f t="shared" si="20"/>
         <v>0</v>
       </c>
@@ -3635,11 +3636,11 @@
       </c>
       <c r="AX26" s="42"/>
       <c r="AY26" s="42"/>
-      <c r="AZ26" s="31">
-        <f>SUM(AZ14:AZ25)</f>
-        <v>0</v>
-      </c>
-      <c r="BA26" s="32">
+      <c r="AZ26" s="40">
+        <f>ROUND(SUM(AZ14:AZ25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="BA26" s="31">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
@@ -3648,11 +3649,11 @@
       </c>
       <c r="BD26" s="42"/>
       <c r="BE26" s="42"/>
-      <c r="BF26" s="31">
-        <f>SUM(BF14:BF25)</f>
-        <v>0</v>
-      </c>
-      <c r="BG26" s="33">
+      <c r="BF26" s="40">
+        <f>ROUND(SUM(BF14:BF25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="BG26" s="32">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -3661,11 +3662,11 @@
       </c>
       <c r="BJ26" s="42"/>
       <c r="BK26" s="42"/>
-      <c r="BL26" s="31">
-        <f>SUM(BL14:BL25)</f>
-        <v>0</v>
-      </c>
-      <c r="BM26" s="33">
+      <c r="BL26" s="40">
+        <f>ROUND(SUM(BL14:BL25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="BM26" s="32">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -3674,11 +3675,11 @@
       </c>
       <c r="BP26" s="42"/>
       <c r="BQ26" s="42"/>
-      <c r="BR26" s="31">
-        <f>SUM(BR14:BR25)</f>
-        <v>0</v>
-      </c>
-      <c r="BS26" s="33">
+      <c r="BR26" s="40">
+        <f>ROUND(SUM(BR14:BR25),2)</f>
+        <v>0</v>
+      </c>
+      <c r="BS26" s="32">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -3704,7 +3705,7 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F28" s="34"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="2:71" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
@@ -3789,7 +3790,7 @@
       </c>
       <c r="C36" s="42"/>
       <c r="D36" s="42"/>
-      <c r="E36" s="35">
+      <c r="E36" s="34">
         <f>SUM(E14:E35)</f>
         <v>0</v>
       </c>

</xml_diff>